<commit_message>
Adding Screws for Servos
resolution to https://github.com/robomechanics/MiniRHex/issues/1
</commit_message>
<xml_diff>
--- a/HardwareList/MiniRhexHardware.xlsx
+++ b/HardwareList/MiniRhexHardware.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Monica/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joepayne/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1108DAF5-CFE0-874F-88BF-7121AA154D2B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Item</t>
   </si>
@@ -102,12 +103,18 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/#93657a212/=1cvg4m2</t>
+  </si>
+  <si>
+    <t>Servo Screws</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92005a078</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -172,6 +179,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -439,11 +449,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,14 +543,14 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2">
-        <v>4.25</v>
+        <v>5.9</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -550,14 +560,14 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>131.4</v>
+        <v>4.25</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -567,14 +577,14 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>23.79</v>
+        <v>131.4</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -584,14 +594,14 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2">
-        <v>6.49</v>
+        <v>23.79</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -601,14 +611,14 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
-        <v>5.73</v>
+        <v>6.49</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -618,14 +628,14 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>9.84</v>
+        <v>5.73</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -635,14 +645,14 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2">
-        <v>32.9</v>
+        <v>9.84</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -652,14 +662,14 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2">
-        <v>5.4</v>
+        <v>32.9</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -668,29 +678,47 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>5.4</v>
+      </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4" location="92005a076/=1cvfwje"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D10" r:id="rId8" location="acrylic/=1cvfzgg"/>
-    <hyperlink ref="D11" r:id="rId9" location="93625a102/=1cvfxju"/>
-    <hyperlink ref="D12" r:id="rId10"/>
-    <hyperlink ref="D13" r:id="rId11" location="93657a212/=1cvg4m2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D7" r:id="rId4" location="92005a076/=1cvfwje" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D11" r:id="rId8" location="acrylic/=1cvfzgg" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D12" r:id="rId9" location="93625a102/=1cvfxju" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D14" r:id="rId11" location="93657a212/=1cvg4m2" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D6" r:id="rId12" xr:uid="{A6E84D68-7FA3-E646-A081-847D8C1A3582}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>